<commit_message>
changed file list excel
</commit_message>
<xml_diff>
--- a/excel_files/file_list_table.xlsx
+++ b/excel_files/file_list_table.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16300" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16300" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,9 +42,6 @@
     <t>sheet location</t>
   </si>
   <si>
-    <t>/Users/krishanuroy/Desktop/Files</t>
-  </si>
-  <si>
     <t>|</t>
   </si>
   <si>
@@ -76,6 +73,9 @@
   </si>
   <si>
     <t>specify database field</t>
+  </si>
+  <si>
+    <t>${SOURCE_FILE_PATH}</t>
   </si>
 </sst>
 </file>
@@ -392,8 +392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -412,25 +412,25 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
       <c r="F1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -438,26 +438,26 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" t="str">
         <f>variables!A2&amp;"/file1.csv"</f>
-        <v>/Users/krishanuroy/Desktop/Files/file1.csv</v>
+        <v>${SOURCE_FILE_PATH}/file1.csv</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -469,8 +469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -485,7 +485,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>